<commit_message>
MTK still not working for large system
</commit_message>
<xml_diff>
--- a/examples/ParsingDiagnostics.xlsx
+++ b/examples/ParsingDiagnostics.xlsx
@@ -142,31 +142,31 @@
     <t>RFeSH2S = kFeSH2S*FeS*TH2S</t>
   </si>
   <si>
-    <t>RFeS_dis = (-tanh.(100.0*(Omega_RFeS_dis - 1.0))/2+0.5) * (kFeSdis*FeS*(1-Omega_RFeS_dis))</t>
-  </si>
-  <si>
-    <t>RFeS_pre = (tanh.(100.0*(Omega_RFeS_pre - 1.0))/2+0.5) * (kFeSpre*Fe*TH2S*(Omega_RFeS_pre-1))</t>
-  </si>
-  <si>
-    <t>RCaCO3_dis = (-tanh.(100.0*(Omega_RCaCO3_dis - 1.0))/2+0.5) * (kCaCO3dis0*CaCO3+kCaCO3dis1*CaCO3*(1-Omega_RCaCO3_dis)^nCaCO3dis)</t>
-  </si>
-  <si>
-    <t>RCaCO3_pre = (tanh.(100.0*(Omega_RCaCO3_pre - 1.0))/2+0.5) * (kCaCO3pre*CaCO3*(Omega_RCaCO3_pre-1))</t>
-  </si>
-  <si>
-    <t>RMnCO3_dis = (-tanh.(100.0*(Omega_RMnCO3_dis - 1.0))/2+0.5) * (kMnCO3dis*MnCO3*(1-Omega_RMnCO3_dis))</t>
-  </si>
-  <si>
-    <t>RMnCO3_pre = (tanh.(100.0*(Omega_RMnCO3_pre - 1.0))/2+0.5) * (kMnCO3pre*(Omega_RMnCO3_pre-1))</t>
-  </si>
-  <si>
-    <t>RFeCO3_dis = (-tanh.(100.0*(Omega_RFeCO3_dis - 1.0))/2+0.5) * (kFeCO3dis*FeCO3*(1-Omega_RFeCO3_dis))</t>
-  </si>
-  <si>
-    <t>RFeCO3_pre = (tanh.(100.0*(Omega_RFeCO3_pre - 1.0))/2+0.5) * (kFeCO3pre*(Omega_RFeCO3_pre-1))</t>
-  </si>
-  <si>
-    <t>RBSi_dis = (-tanh.(100.0*(Omega_RBSi_dis - 1.0))/2+0.5) * ((1-Omega_RBSi_dis)*BSi*nuBSi/(aBSi+Age))</t>
+    <t>RFeS_dis = (-tanh(100.0*(Omega_RFeS_dis - 1.0))/2+0.5) * (kFeSdis*FeS*(1-Omega_RFeS_dis))</t>
+  </si>
+  <si>
+    <t>RFeS_pre = (tanh(100.0*(Omega_RFeS_pre - 1.0))/2+0.5) * (kFeSpre*Fe*TH2S*(Omega_RFeS_pre-1))</t>
+  </si>
+  <si>
+    <t>RCaCO3_dis = (-tanh(100.0*(Omega_RCaCO3_dis - 1.0))/2+0.5) * (kCaCO3dis0*CaCO3+kCaCO3dis1*CaCO3*(1-Omega_RCaCO3_dis)^nCaCO3dis)</t>
+  </si>
+  <si>
+    <t>RCaCO3_pre = (tanh(100.0*(Omega_RCaCO3_pre - 1.0))/2+0.5) * (kCaCO3pre*CaCO3*(Omega_RCaCO3_pre-1))</t>
+  </si>
+  <si>
+    <t>RMnCO3_dis = (-tanh(100.0*(Omega_RMnCO3_dis - 1.0))/2+0.5) * (kMnCO3dis*MnCO3*(1-Omega_RMnCO3_dis))</t>
+  </si>
+  <si>
+    <t>RMnCO3_pre = (tanh(100.0*(Omega_RMnCO3_pre - 1.0))/2+0.5) * (kMnCO3pre*(Omega_RMnCO3_pre-1))</t>
+  </si>
+  <si>
+    <t>RFeCO3_dis = (-tanh(100.0*(Omega_RFeCO3_dis - 1.0))/2+0.5) * (kFeCO3dis*FeCO3*(1-Omega_RFeCO3_dis))</t>
+  </si>
+  <si>
+    <t>RFeCO3_pre = (tanh(100.0*(Omega_RFeCO3_pre - 1.0))/2+0.5) * (kFeCO3pre*(Omega_RFeCO3_pre-1))</t>
+  </si>
+  <si>
+    <t>RBSi_dis = (-tanh(100.0*(Omega_RBSi_dis - 1.0))/2+0.5) * ((1-Omega_RBSi_dis)*BSi*nuBSi/(aBSi+Age))</t>
   </si>
   <si>
     <t>RMnO2POC_Nd = RMnO2POC*2</t>
@@ -193,10 +193,10 @@
     <t>RO2Fe_Ndr = RO2Fe*rNdnrFe*Ndr/Ndnr</t>
   </si>
   <si>
-    <t>RNdnrPO4_pre = (tanh.(100.0*(Omega_RNdnrPO4_pre - 1.0))/2+0.5) * (kNdPO4_pre*fNdnr*(Omega_RNdnrPO4_pre-1))</t>
-  </si>
-  <si>
-    <t>RNdrPO4_pre = (tanh.(100.0*(Omega_RNdrPO4_pre - 1.0))/2+0.5) * (kNdPO4_pre*Ndr/Ndnr*fNdnr*(Omega_RNdrPO4_pre-1))</t>
+    <t>RNdnrPO4_pre = (tanh(100.0*(Omega_RNdnrPO4_pre - 1.0))/2+0.5) * (kNdPO4_pre*fNdnr*(Omega_RNdnrPO4_pre-1))</t>
+  </si>
+  <si>
+    <t>RNdrPO4_pre = (tanh(100.0*(Omega_RNdrPO4_pre - 1.0))/2+0.5) * (kNdPO4_pre*Ndr/Ndnr*fNdnr*(Omega_RNdrPO4_pre-1))</t>
   </si>
   <si>
     <t># species rates</t>
@@ -313,7 +313,7 @@
     <t>S_H = S_H/dTA_dH</t>
   </si>
   <si>
-    <t>S_Age = ones(Ngrid)</t>
+    <t>S_Age = 1</t>
   </si>
   <si>
     <t>label</t>

</xml_diff>